<commit_message>
Option to print all in directory
</commit_message>
<xml_diff>
--- a/templateOld.xlsx
+++ b/templateOld.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\TimeSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049070A5-D490-449B-B3D6-152410B75B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B00F3D9-7EC2-49D5-B0F8-2FA3A58308AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="999" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>PARTICIPANT SIGN IN SHEET      签到表</t>
   </si>
@@ -88,34 +88,22 @@
     <t>Day</t>
   </si>
   <si>
-    <t xml:space="preserve">NAME (姓名): </t>
-  </si>
-  <si>
-    <t>DIA CODE: M15.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PARTICIPANT ADDRESS: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEL: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOB: </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ID #: IT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GENDER: </t>
-  </si>
-  <si>
     <t>MON    TUE    WED    THU</t>
   </si>
   <si>
     <t>VERY GOOD BUILDING COMPANY</t>
   </si>
   <si>
-    <t xml:space="preserve">MLTC INSURANCE (保险公司): </t>
+    <t>星期一</t>
+  </si>
+  <si>
+    <t>星期二</t>
+  </si>
+  <si>
+    <t>星期三</t>
+  </si>
+  <si>
+    <t>星期四</t>
   </si>
 </sst>
 </file>
@@ -123,8 +111,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
-    <numFmt numFmtId="167" formatCode="[$-804]aaaa;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="165" formatCode="[$-804]aaaa;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -184,7 +172,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -216,11 +204,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -245,20 +248,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -275,101 +274,25 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <border>
         <left style="thin">
@@ -603,7 +526,7 @@
   <dimension ref="A1:H964"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:H5"/>
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -617,7 +540,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="16" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -650,27 +573,17 @@
       <c r="H3" s="17"/>
     </row>
     <row r="4" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="18" t="s">
-        <v>16</v>
-      </c>
+      <c r="A4" s="18"/>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
-      <c r="D4" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>19</v>
-      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="22"/>
       <c r="F4" s="22"/>
-      <c r="G4" s="21" t="s">
-        <v>22</v>
-      </c>
+      <c r="G4" s="21"/>
       <c r="H4" s="21"/>
     </row>
     <row r="5" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="23" t="s">
-        <v>18</v>
-      </c>
+      <c r="A5" s="23"/>
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -680,30 +593,24 @@
       <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="A6" s="18"/>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
-      <c r="D6" s="11" t="s">
-        <v>21</v>
-      </c>
+      <c r="D6" s="10"/>
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="23" t="s">
-        <v>17</v>
-      </c>
+      <c r="A7" s="23"/>
       <c r="B7" s="23"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="22"/>
       <c r="F7" s="22"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
@@ -711,10 +618,10 @@
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="18" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D8" s="19"/>
-      <c r="E8" s="11"/>
+      <c r="E8" s="10"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="7"/>
@@ -722,7 +629,7 @@
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
-      <c r="C9" s="12"/>
+      <c r="C9" s="11"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
@@ -778,156 +685,366 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="13"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="A12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="13">
+        <v>45413</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="13"/>
-      <c r="B13" s="10"/>
+      <c r="A13" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="13">
+        <v>45414</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
-      <c r="B14" s="10"/>
+      <c r="A14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="13">
+        <v>45418</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="13"/>
-      <c r="B15" s="10"/>
+      <c r="A15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="13">
+        <v>45419</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="13"/>
-      <c r="B16" s="10"/>
-    </row>
-    <row r="17" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="13"/>
-      <c r="B17" s="10"/>
-    </row>
-    <row r="18" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="13"/>
-      <c r="B18" s="10"/>
-    </row>
-    <row r="19" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="13"/>
-      <c r="B19" s="10"/>
-    </row>
-    <row r="20" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="13"/>
-      <c r="B20" s="10"/>
-    </row>
-    <row r="21" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="13"/>
-      <c r="B21" s="10"/>
-    </row>
-    <row r="22" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="13"/>
-      <c r="B22" s="10"/>
-    </row>
-    <row r="23" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="13"/>
-      <c r="B23" s="10"/>
-    </row>
-    <row r="24" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="13"/>
-      <c r="B24" s="10"/>
-    </row>
-    <row r="25" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="13"/>
-      <c r="B25" s="10"/>
-    </row>
-    <row r="26" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="13"/>
-      <c r="B26" s="10"/>
-    </row>
-    <row r="27" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="13"/>
-      <c r="B27" s="10"/>
-    </row>
-    <row r="28" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="13"/>
-      <c r="B28" s="10"/>
-    </row>
-    <row r="29" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="13"/>
-      <c r="B29" s="10"/>
-    </row>
-    <row r="30" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="13"/>
-      <c r="B30" s="10"/>
-    </row>
-    <row r="31" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="15"/>
-      <c r="B31" s="10"/>
-    </row>
-    <row r="32" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="15"/>
-      <c r="B32" s="10"/>
+      <c r="A16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="13">
+        <v>45420</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+    </row>
+    <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="13">
+        <v>45421</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="13">
+        <v>45425</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+    </row>
+    <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="13">
+        <v>45426</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+    </row>
+    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="13">
+        <v>45427</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+    </row>
+    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="13">
+        <v>45428</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+    </row>
+    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="13">
+        <v>45432</v>
+      </c>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="13">
+        <v>45433</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+    </row>
+    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="13">
+        <v>45434</v>
+      </c>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+    </row>
+    <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="13">
+        <v>45435</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+    </row>
+    <row r="26" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="13">
+        <v>45439</v>
+      </c>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+    </row>
+    <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="13">
+        <v>45440</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="13">
+        <v>45441</v>
+      </c>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+    </row>
+    <row r="29" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="13">
+        <v>45442</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+    </row>
+    <row r="30" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="24"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+    </row>
+    <row r="31" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="28"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+    </row>
+    <row r="32" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="28"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
     </row>
     <row r="33" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="15"/>
-      <c r="B33" s="10"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
     </row>
     <row r="34" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="13"/>
-      <c r="B34" s="14"/>
+      <c r="A34" s="24"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
     </row>
     <row r="35" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="15"/>
-      <c r="B35" s="10"/>
+      <c r="A35" s="28"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
     </row>
     <row r="36" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="15"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
+      <c r="A36" s="28"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
     </row>
     <row r="37" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="15"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
+      <c r="A37" s="28"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
     </row>
     <row r="38" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="15"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
+      <c r="A38" s="28"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
     </row>
     <row r="39" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="15"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
+      <c r="A39" s="28"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
     </row>
     <row r="40" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="15"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
+      <c r="A40" s="28"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
     </row>
     <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3717,7 +3834,7 @@
     <mergeCell ref="E7:F7"/>
   </mergeCells>
   <conditionalFormatting sqref="A34">
-    <cfRule type="expression" dxfId="2" priority="88">
+    <cfRule type="expression" dxfId="0" priority="88">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>